<commit_message>
Dealing with PEI input contstrains
</commit_message>
<xml_diff>
--- a/tests/circulator-import-test.xlsx
+++ b/tests/circulator-import-test.xlsx
@@ -1413,13 +1413,13 @@
   </sheetPr>
   <dimension ref="A1:AL21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Y1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Y8" activeCellId="0" sqref="7:8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AB1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AI6" activeCellId="0" sqref="AI6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.85"/>
@@ -1873,7 +1873,7 @@
         <v>150</v>
       </c>
       <c r="AI5" s="0" t="n">
-        <v>1.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3030,7 +3030,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E21" activeCellId="1" sqref="7:8 E21"/>
+      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Enabled circulators email attachment for subscribers
</commit_message>
<xml_diff>
--- a/tests/circulator-import-test.xlsx
+++ b/tests/circulator-import-test.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="124">
   <si>
     <t xml:space="preserve">Pump Characteristics</t>
   </si>
@@ -577,6 +577,9 @@
     <t xml:space="preserve">CP3: Dry Rotor Three Piece</t>
   </si>
   <si>
+    <t xml:space="preserve">000106</t>
+  </si>
+  <si>
     <t xml:space="preserve">Yes</t>
   </si>
   <si>
@@ -680,8 +683,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -1057,7 +1061,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1323,6 +1327,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1413,8 +1421,8 @@
   </sheetPr>
   <dimension ref="A1:AL21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AB1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AI6" activeCellId="0" sqref="AI6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1826,23 +1834,23 @@
       <c r="F5" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="G5" s="0" t="n">
-        <v>8</v>
+      <c r="G5" s="67" t="s">
+        <v>90</v>
       </c>
       <c r="H5" s="66" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I5" s="66" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="J5" s="66" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K5" s="66"/>
       <c r="L5" s="66"/>
       <c r="M5" s="66"/>
       <c r="N5" s="66" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="O5" s="66"/>
       <c r="R5" s="0" t="n">
@@ -1884,43 +1892,43 @@
         <v>86</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>43</v>
       </c>
       <c r="F6" s="66" t="s">
-        <v>94</v>
-      </c>
-      <c r="G6" s="0" t="n">
-        <v>8</v>
+        <v>95</v>
+      </c>
+      <c r="G6" s="67" t="s">
+        <v>90</v>
       </c>
       <c r="H6" s="66"/>
       <c r="I6" s="66" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="J6" s="66" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K6" s="66"/>
       <c r="L6" s="66" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="M6" s="66"/>
       <c r="N6" s="66" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O6" s="66" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="P6" s="66" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="Q6" s="66" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="R6" s="0" t="n">
         <v>0.4</v>
@@ -1968,161 +1976,161 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="7" s="67" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="67" t="s">
+    <row r="7" s="68" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="68" t="s">
         <v>85</v>
       </c>
-      <c r="B7" s="67" t="s">
+      <c r="B7" s="68" t="s">
         <v>86</v>
       </c>
-      <c r="C7" s="67" t="s">
-        <v>99</v>
-      </c>
-      <c r="D7" s="67" t="s">
+      <c r="C7" s="68" t="s">
         <v>100</v>
       </c>
-      <c r="E7" s="67" t="n">
+      <c r="D7" s="68" t="s">
+        <v>101</v>
+      </c>
+      <c r="E7" s="68" t="n">
         <v>44</v>
       </c>
-      <c r="F7" s="67" t="s">
-        <v>101</v>
-      </c>
-      <c r="G7" s="67" t="n">
-        <v>8</v>
-      </c>
-      <c r="H7" s="68"/>
-      <c r="I7" s="68" t="s">
+      <c r="F7" s="68" t="s">
+        <v>102</v>
+      </c>
+      <c r="G7" s="67" t="s">
         <v>90</v>
       </c>
-      <c r="J7" s="68"/>
-      <c r="K7" s="68"/>
-      <c r="L7" s="68"/>
-      <c r="M7" s="68" t="s">
+      <c r="H7" s="69"/>
+      <c r="I7" s="69" t="s">
+        <v>91</v>
+      </c>
+      <c r="J7" s="69"/>
+      <c r="K7" s="69"/>
+      <c r="L7" s="69"/>
+      <c r="M7" s="69" t="s">
+        <v>91</v>
+      </c>
+      <c r="N7" s="68" t="s">
+        <v>96</v>
+      </c>
+      <c r="O7" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="R7" s="68" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="S7" s="68" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="T7" s="68" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="U7" s="68" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="AB7" s="68" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="AC7" s="68" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="AD7" s="68" t="n">
+        <v>17</v>
+      </c>
+      <c r="AE7" s="68" t="n">
+        <v>23</v>
+      </c>
+      <c r="AF7" s="68" t="n">
+        <v>33</v>
+      </c>
+      <c r="AG7" s="68" t="n">
+        <v>40</v>
+      </c>
+      <c r="AH7" s="68" t="n">
+        <v>150</v>
+      </c>
+      <c r="AI7" s="68" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="AJ7" s="68" t="n">
+        <v>1.74</v>
+      </c>
+    </row>
+    <row r="8" s="68" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="68" t="s">
+        <v>85</v>
+      </c>
+      <c r="B8" s="68" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" s="68" t="s">
+        <v>104</v>
+      </c>
+      <c r="D8" s="68" t="s">
+        <v>105</v>
+      </c>
+      <c r="E8" s="68" t="n">
+        <v>45</v>
+      </c>
+      <c r="F8" s="68" t="s">
+        <v>102</v>
+      </c>
+      <c r="G8" s="67" t="s">
         <v>90</v>
       </c>
-      <c r="N7" s="67" t="s">
-        <v>95</v>
-      </c>
-      <c r="O7" s="67" t="s">
-        <v>102</v>
-      </c>
-      <c r="R7" s="67" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="S7" s="67" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="T7" s="67" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="U7" s="67" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="AB7" s="67" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="AC7" s="67" t="n">
+      <c r="H8" s="69"/>
+      <c r="I8" s="69" t="s">
+        <v>91</v>
+      </c>
+      <c r="J8" s="69"/>
+      <c r="K8" s="69" t="s">
+        <v>91</v>
+      </c>
+      <c r="L8" s="69"/>
+      <c r="M8" s="69" t="s">
+        <v>91</v>
+      </c>
+      <c r="N8" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="O8" s="68" t="s">
+        <v>96</v>
+      </c>
+      <c r="V8" s="68" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="W8" s="68" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="X8" s="68" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="Y8" s="68" t="n">
         <v>1.4</v>
       </c>
-      <c r="AD7" s="67" t="n">
+      <c r="Z8" s="68" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="AA8" s="68" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="AD8" s="68" t="n">
         <v>17</v>
       </c>
-      <c r="AE7" s="67" t="n">
+      <c r="AE8" s="68" t="n">
         <v>23</v>
       </c>
-      <c r="AF7" s="67" t="n">
+      <c r="AF8" s="68" t="n">
         <v>33</v>
       </c>
-      <c r="AG7" s="67" t="n">
+      <c r="AG8" s="68" t="n">
         <v>40</v>
       </c>
-      <c r="AH7" s="67" t="n">
+      <c r="AH8" s="68" t="n">
         <v>150</v>
       </c>
-      <c r="AI7" s="67" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="AJ7" s="67" t="n">
-        <v>1.74</v>
-      </c>
-    </row>
-    <row r="8" s="67" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="67" t="s">
-        <v>85</v>
-      </c>
-      <c r="B8" s="67" t="s">
-        <v>86</v>
-      </c>
-      <c r="C8" s="67" t="s">
-        <v>103</v>
-      </c>
-      <c r="D8" s="67" t="s">
-        <v>104</v>
-      </c>
-      <c r="E8" s="67" t="n">
-        <v>45</v>
-      </c>
-      <c r="F8" s="67" t="s">
-        <v>101</v>
-      </c>
-      <c r="G8" s="67" t="n">
-        <v>8</v>
-      </c>
-      <c r="H8" s="68"/>
-      <c r="I8" s="68" t="s">
-        <v>90</v>
-      </c>
-      <c r="J8" s="68"/>
-      <c r="K8" s="68" t="s">
-        <v>90</v>
-      </c>
-      <c r="L8" s="68"/>
-      <c r="M8" s="68" t="s">
-        <v>90</v>
-      </c>
-      <c r="N8" s="67" t="s">
-        <v>102</v>
-      </c>
-      <c r="O8" s="67" t="s">
-        <v>95</v>
-      </c>
-      <c r="V8" s="67" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="W8" s="67" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="X8" s="67" t="n">
-        <v>0.65</v>
-      </c>
-      <c r="Y8" s="67" t="n">
-        <v>1.4</v>
-      </c>
-      <c r="Z8" s="67" t="n">
-        <v>2.6</v>
-      </c>
-      <c r="AA8" s="67" t="n">
-        <v>3.2</v>
-      </c>
-      <c r="AD8" s="67" t="n">
-        <v>17</v>
-      </c>
-      <c r="AE8" s="67" t="n">
-        <v>23</v>
-      </c>
-      <c r="AF8" s="67" t="n">
-        <v>33</v>
-      </c>
-      <c r="AG8" s="67" t="n">
-        <v>40</v>
-      </c>
-      <c r="AH8" s="67" t="n">
-        <v>150</v>
-      </c>
-      <c r="AI8" s="67" t="n">
+      <c r="AI8" s="68" t="n">
         <v>1.15</v>
       </c>
-      <c r="AJ8" s="67" t="n">
+      <c r="AJ8" s="68" t="n">
         <v>1.7</v>
       </c>
     </row>
@@ -2134,19 +2142,19 @@
         <v>86</v>
       </c>
       <c r="C9" s="66" t="s">
+        <v>106</v>
+      </c>
+      <c r="D9" s="66" t="s">
         <v>105</v>
-      </c>
-      <c r="D9" s="66" t="s">
-        <v>104</v>
       </c>
       <c r="E9" s="66" t="n">
         <v>45</v>
       </c>
       <c r="F9" s="66" t="s">
-        <v>101</v>
-      </c>
-      <c r="G9" s="66" t="n">
-        <v>8</v>
+        <v>102</v>
+      </c>
+      <c r="G9" s="67" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="10" s="66" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2157,22 +2165,22 @@
         <v>86</v>
       </c>
       <c r="C10" s="66" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D10" s="66" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E10" s="66" t="n">
         <v>45</v>
       </c>
       <c r="F10" s="66" t="s">
-        <v>101</v>
-      </c>
-      <c r="G10" s="66" t="n">
-        <v>8</v>
+        <v>102</v>
+      </c>
+      <c r="G10" s="67" t="s">
+        <v>90</v>
       </c>
       <c r="N10" s="66" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="R10" s="66" t="n">
         <v>0.4</v>
@@ -2213,25 +2221,25 @@
         <v>86</v>
       </c>
       <c r="C11" s="66" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D11" s="66" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E11" s="66" t="n">
         <v>45</v>
       </c>
       <c r="F11" s="66" t="s">
-        <v>101</v>
-      </c>
-      <c r="G11" s="66" t="n">
-        <v>8</v>
+        <v>102</v>
+      </c>
+      <c r="G11" s="67" t="s">
+        <v>90</v>
       </c>
       <c r="J11" s="66" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="N11" s="66" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="R11" s="66" t="n">
         <v>0.4</v>
@@ -2272,31 +2280,31 @@
         <v>86</v>
       </c>
       <c r="C12" s="66" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D12" s="66" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E12" s="66" t="n">
         <v>45</v>
       </c>
       <c r="F12" s="66" t="s">
-        <v>101</v>
-      </c>
-      <c r="G12" s="66" t="n">
-        <v>8</v>
+        <v>102</v>
+      </c>
+      <c r="G12" s="67" t="s">
+        <v>90</v>
       </c>
       <c r="I12" s="66" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="J12" s="66" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="N12" s="66" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O12" s="66" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="R12" s="66" t="n">
         <v>0.4</v>
@@ -2346,34 +2354,34 @@
         <v>86</v>
       </c>
       <c r="C13" s="66" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D13" s="66" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E13" s="66" t="n">
         <v>45</v>
       </c>
       <c r="F13" s="66" t="s">
-        <v>101</v>
-      </c>
-      <c r="G13" s="66" t="n">
-        <v>8</v>
+        <v>102</v>
+      </c>
+      <c r="G13" s="67" t="s">
+        <v>90</v>
       </c>
       <c r="I13" s="66" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="J13" s="66" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="M13" s="66" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="N13" s="66" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O13" s="66" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="R13" s="66" t="n">
         <v>0.4</v>
@@ -2420,34 +2428,34 @@
         <v>86</v>
       </c>
       <c r="C14" s="66" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D14" s="66" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E14" s="66" t="n">
         <v>45</v>
       </c>
       <c r="F14" s="66" t="s">
-        <v>101</v>
-      </c>
-      <c r="G14" s="66" t="n">
-        <v>8</v>
+        <v>102</v>
+      </c>
+      <c r="G14" s="67" t="s">
+        <v>90</v>
       </c>
       <c r="I14" s="66" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="J14" s="66" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="M14" s="66" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="N14" s="66" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O14" s="66" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="R14" s="66" t="n">
         <v>0.4</v>
@@ -2468,7 +2476,7 @@
         <v>1.4</v>
       </c>
       <c r="AD14" s="66" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="AE14" s="66" t="n">
         <v>23</v>
@@ -2497,31 +2505,31 @@
         <v>86</v>
       </c>
       <c r="C15" s="66" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D15" s="66" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E15" s="66" t="n">
         <v>44</v>
       </c>
       <c r="F15" s="66" t="s">
-        <v>101</v>
-      </c>
-      <c r="G15" s="66" t="n">
-        <v>8</v>
+        <v>102</v>
+      </c>
+      <c r="G15" s="67" t="s">
+        <v>90</v>
       </c>
       <c r="I15" s="66" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="M15" s="66" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="N15" s="66" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O15" s="66" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="R15" s="66" t="n">
         <v>0.4</v>
@@ -2554,7 +2562,7 @@
         <v>40</v>
       </c>
       <c r="AH15" s="66" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AI15" s="66" t="n">
         <v>1.3</v>
@@ -2571,31 +2579,31 @@
         <v>86</v>
       </c>
       <c r="C16" s="66" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D16" s="66" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E16" s="66" t="n">
         <v>44</v>
       </c>
       <c r="F16" s="66" t="s">
-        <v>101</v>
-      </c>
-      <c r="G16" s="66" t="n">
-        <v>8</v>
+        <v>102</v>
+      </c>
+      <c r="G16" s="67" t="s">
+        <v>90</v>
       </c>
       <c r="I16" s="66" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="M16" s="66" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="N16" s="66" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O16" s="66" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="R16" s="66" t="n">
         <v>0.4</v>
@@ -2642,31 +2650,31 @@
         <v>86</v>
       </c>
       <c r="C17" s="66" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D17" s="66" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E17" s="66" t="n">
         <v>44</v>
       </c>
       <c r="F17" s="66" t="s">
-        <v>101</v>
-      </c>
-      <c r="G17" s="66" t="n">
-        <v>8</v>
+        <v>102</v>
+      </c>
+      <c r="G17" s="67" t="s">
+        <v>90</v>
       </c>
       <c r="I17" s="66" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="M17" s="66" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="N17" s="66" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O17" s="66" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="R17" s="66" t="n">
         <v>0.4</v>
@@ -2705,7 +2713,7 @@
         <v>1.3</v>
       </c>
       <c r="AJ17" s="66" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18" s="66" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2716,7 +2724,7 @@
         <v>86</v>
       </c>
       <c r="C18" s="66" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D18" s="66" t="s">
         <v>88</v>
@@ -2727,20 +2735,20 @@
       <c r="F18" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="G18" s="66" t="n">
-        <v>8</v>
+      <c r="G18" s="67" t="s">
+        <v>90</v>
       </c>
       <c r="H18" s="66" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I18" s="66" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="J18" s="66" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="N18" s="66" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="V18" s="66" t="n">
         <v>1.9</v>
@@ -2775,7 +2783,7 @@
         <v>86</v>
       </c>
       <c r="C19" s="66" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D19" s="66" t="s">
         <v>88</v>
@@ -2786,23 +2794,23 @@
       <c r="F19" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="G19" s="66" t="n">
-        <v>8</v>
+      <c r="G19" s="67" t="s">
+        <v>90</v>
       </c>
       <c r="H19" s="66" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I19" s="66" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="J19" s="66" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="M19" s="66" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="N19" s="66" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="R19" s="66" t="n">
         <v>0.4</v>
@@ -2843,34 +2851,34 @@
         <v>86</v>
       </c>
       <c r="C20" s="66" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D20" s="66" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E20" s="66" t="n">
         <v>45</v>
       </c>
       <c r="F20" s="66" t="s">
-        <v>101</v>
-      </c>
-      <c r="G20" s="66" t="n">
-        <v>8</v>
+        <v>102</v>
+      </c>
+      <c r="G20" s="67" t="s">
+        <v>90</v>
       </c>
       <c r="I20" s="66" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K20" s="66" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="M20" s="66" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="N20" s="66" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="O20" s="66" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="V20" s="66" t="n">
         <v>1.5</v>
@@ -2914,34 +2922,34 @@
         <v>86</v>
       </c>
       <c r="C21" s="66" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D21" s="66" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E21" s="66" t="n">
         <v>45</v>
       </c>
       <c r="F21" s="66" t="s">
-        <v>101</v>
-      </c>
-      <c r="G21" s="66" t="n">
-        <v>8</v>
+        <v>102</v>
+      </c>
+      <c r="G21" s="67" t="s">
+        <v>90</v>
       </c>
       <c r="I21" s="66" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K21" s="66" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="M21" s="66" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="N21" s="66" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="O21" s="66" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="V21" s="66" t="n">
         <v>1.5</v>
@@ -3030,7 +3038,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
+      <selection pane="topLeft" activeCell="E21" activeCellId="1" sqref="G21 E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3042,26 +3050,26 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>95</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>89</v>
@@ -3069,17 +3077,17 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>